<commit_message>
Update edited session - 2025-08-14T07:14:29.565Z - Cache Bust: 1755155669565
</commit_message>
<xml_diff>
--- a/log_history/Y1_B2223_Anatomy_scanner1755155582835_5edfa2692bdacc5e6ee805c626c50cb44cebb065f092d9a1067d89f74dacd326.xlsx
+++ b/log_history/Y1_B2223_Anatomy_scanner1755155582835_5edfa2692bdacc5e6ee805c626c50cb44cebb065f092d9a1067d89f74dacd326.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Scanner" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -439,32 +439,12 @@
         <v>Manual</v>
       </c>
       <c r="F2" t="str">
-        <v>admin@admin.com</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>654321</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Anatomy</v>
-      </c>
-      <c r="C3" t="str">
-        <v>14/08/2025</v>
-      </c>
-      <c r="D3" t="str">
-        <v>10:13:08</v>
-      </c>
-      <c r="E3" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F3" t="str">
-        <v>admin@admin.com</v>
+        <v>5edfa2692bdacc5e6ee805c626c50cb44cebb065f092d9a1067d89f74dacd326</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>